<commit_message>
afficher tableau mission pour selectionner mission a afficher son plan de chargement. adapter le plan de chargement du version 0
</commit_message>
<xml_diff>
--- a/src/assets/DATA/20-01-2022/BL/3.xlsx
+++ b/src/assets/DATA/20-01-2022/BL/3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DATA\20-01-2022\BL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC279FD8-1F06-45FE-A6EC-A7D20673C7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C88CEEA-CCD3-40D6-8CCC-A6DB31348DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,7 +466,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>